<commit_message>
Done Order Mgmt, Order details, Stock Mgmt, Edit address, Return Product, Eslint coding std
</commit_message>
<xml_diff>
--- a/public/files/SalesReport.xlsx
+++ b/public/files/SalesReport.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,39 +412,31 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>CiFi Beer</v>
+        <v>Airén</v>
       </c>
       <c r="B2">
-        <v>7700</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>New Cometa</v>
+        <v>New cometa</v>
       </c>
       <c r="B3">
-        <v>3300</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Chakras Wine</v>
+        <v>Cometa</v>
       </c>
       <c r="B4">
-        <v>6670</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v xml:space="preserve">Cometa </v>
-      </c>
-      <c r="B5">
-        <v>7800</v>
+        <v>1300</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>